<commit_message>
Fixed all the small issues of this project
</commit_message>
<xml_diff>
--- a/processed_files/csv_extracted.xlsx
+++ b/processed_files/csv_extracted.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_business_2023 (2)-read-r" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_business_2023 (2)" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_business_2023_saving (1)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_personal_2023 (1)-read-r" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="transaction_history-2-read-read" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upwork_2023-read-read-read-read" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="amhfcu_personal_2023 (1)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="transaction_history-2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Upwork_2023" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>